<commit_message>
semana 31 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/revision_IRAExt_semanal.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/revision_IRAExt_semanal.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG57"/>
+  <dimension ref="A1:AH58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -523,6 +523,11 @@
           <t>30</t>
         </is>
       </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -630,6 +635,9 @@
       <c r="AG2">
         <v>60</v>
       </c>
+      <c r="AH2">
+        <v>77</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -716,6 +724,9 @@
       <c r="AF3">
         <v>61</v>
       </c>
+      <c r="AH3">
+        <v>72</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -820,6 +831,9 @@
       <c r="AG4">
         <v>1</v>
       </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -927,6 +941,9 @@
       <c r="AG5">
         <v>3</v>
       </c>
+      <c r="AH5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1034,6 +1051,9 @@
       <c r="AG6">
         <v>117</v>
       </c>
+      <c r="AH6">
+        <v>71</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1138,6 +1158,9 @@
       <c r="AG7">
         <v>35</v>
       </c>
+      <c r="AH7">
+        <v>34</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1242,6 +1265,9 @@
       <c r="AG8">
         <v>38</v>
       </c>
+      <c r="AH8">
+        <v>39</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1429,6 +1455,9 @@
       <c r="AG10">
         <v>4</v>
       </c>
+      <c r="AH10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1503,6 +1532,9 @@
       <c r="AB11">
         <v>1</v>
       </c>
+      <c r="AH11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1559,6 +1591,9 @@
       <c r="AG12">
         <v>1</v>
       </c>
+      <c r="AH12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1639,6 +1674,9 @@
       <c r="AE13">
         <v>1</v>
       </c>
+      <c r="AH13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1731,6 +1769,9 @@
       <c r="AG14">
         <v>2</v>
       </c>
+      <c r="AH14">
+        <v>4</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1808,6 +1849,9 @@
       <c r="AF15">
         <v>2</v>
       </c>
+      <c r="AH15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1873,6 +1917,9 @@
       <c r="AG16">
         <v>1</v>
       </c>
+      <c r="AH16">
+        <v>4</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1959,6 +2006,9 @@
       <c r="AG17">
         <v>2</v>
       </c>
+      <c r="AH17">
+        <v>3</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2241,6 +2291,9 @@
       <c r="AG23">
         <v>2</v>
       </c>
+      <c r="AH23">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2297,6 +2350,9 @@
       <c r="AF24">
         <v>1</v>
       </c>
+      <c r="AH24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2404,6 +2460,9 @@
       <c r="AG25">
         <v>65</v>
       </c>
+      <c r="AH25">
+        <v>56</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2626,6 +2685,9 @@
       <c r="AG28">
         <v>15</v>
       </c>
+      <c r="AH28">
+        <v>213</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2730,6 +2792,9 @@
       <c r="AG29">
         <v>0</v>
       </c>
+      <c r="AH29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2837,6 +2902,9 @@
       <c r="AG30">
         <v>23</v>
       </c>
+      <c r="AH30">
+        <v>7</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2944,6 +3012,9 @@
       <c r="AG31">
         <v>4</v>
       </c>
+      <c r="AH31">
+        <v>3</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3051,6 +3122,9 @@
       <c r="AG32">
         <v>8</v>
       </c>
+      <c r="AH32">
+        <v>7</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3121,6 +3195,9 @@
       <c r="AG34">
         <v>3</v>
       </c>
+      <c r="AH34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3228,6 +3305,9 @@
       <c r="AG35">
         <v>39</v>
       </c>
+      <c r="AH35">
+        <v>47</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3335,6 +3415,9 @@
       <c r="AG36">
         <v>1</v>
       </c>
+      <c r="AH36">
+        <v>6</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3439,6 +3522,9 @@
       <c r="AG37">
         <v>10</v>
       </c>
+      <c r="AH37">
+        <v>12</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3546,251 +3632,176 @@
       <c r="AG38">
         <v>92</v>
       </c>
+      <c r="AH38">
+        <v>84</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6600102402</t>
+          <t>6600102288</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>IPS CENTRO DE MEDICINA INTEGRATIVA SAS</t>
-        </is>
-      </c>
-      <c r="Q39">
-        <v>1</v>
-      </c>
-      <c r="S39">
-        <v>4</v>
-      </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
-      <c r="W39">
-        <v>1</v>
-      </c>
-      <c r="X39">
-        <v>1</v>
-      </c>
-      <c r="Y39">
-        <v>3</v>
-      </c>
-      <c r="AB39">
-        <v>4</v>
-      </c>
-      <c r="AC39">
-        <v>5</v>
-      </c>
-      <c r="AD39">
-        <v>2</v>
-      </c>
-      <c r="AE39">
-        <v>3</v>
-      </c>
-      <c r="AF39">
-        <v>1</v>
-      </c>
-      <c r="AG39">
-        <v>1</v>
+          <t>SALUD PYP SAS</t>
+        </is>
+      </c>
+      <c r="AH39">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6600102411</t>
+          <t>6600102402</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SERVICIOS DE SALUD IPS SURAMERICANA SA</t>
-        </is>
-      </c>
-      <c r="I40">
-        <v>1</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>7</v>
-      </c>
-      <c r="M40">
-        <v>22</v>
-      </c>
-      <c r="N40">
-        <v>7</v>
-      </c>
-      <c r="O40">
-        <v>22</v>
-      </c>
-      <c r="P40">
-        <v>8</v>
+          <t>IPS CENTRO DE MEDICINA INTEGRATIVA SAS</t>
+        </is>
       </c>
       <c r="Q40">
-        <v>19</v>
-      </c>
-      <c r="R40">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="S40">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="T40">
-        <v>8</v>
-      </c>
-      <c r="U40">
-        <v>3</v>
-      </c>
-      <c r="V40">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="W40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X40">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="Y40">
-        <v>9</v>
-      </c>
-      <c r="Z40">
-        <v>14</v>
-      </c>
-      <c r="AA40">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AB40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC40">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="AD40">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="AE40">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="AF40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AG40">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="AH40">
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6600102446</t>
+          <t>6600102411</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CAJA COLOMBIANA DE SUBSIDIO FAMILIAR COLSUBSIDIO</t>
-        </is>
-      </c>
-      <c r="D41">
-        <v>56</v>
-      </c>
-      <c r="E41">
-        <v>15</v>
-      </c>
-      <c r="F41">
-        <v>73</v>
-      </c>
-      <c r="G41">
-        <v>82</v>
-      </c>
-      <c r="H41">
-        <v>63</v>
+          <t>SERVICIOS DE SALUD IPS SURAMERICANA SA</t>
+        </is>
       </c>
       <c r="I41">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="J41">
-        <v>73</v>
-      </c>
-      <c r="K41">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="L41">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="M41">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="N41">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="O41">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="P41">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="Q41">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="R41">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="S41">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="T41">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="U41">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="V41">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="W41">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="X41">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="Y41">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="Z41">
-        <v>52</v>
+        <v>14</v>
+      </c>
+      <c r="AA41">
+        <v>10</v>
       </c>
       <c r="AB41">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="AC41">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="AD41">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="AE41">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="AF41">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AG41">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="AH41">
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -3801,7 +3812,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -3810,192 +3821,204 @@
         </is>
       </c>
       <c r="D42">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="E42">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="F42">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="G42">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="H42">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="I42">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="J42">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="K42">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="L42">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="M42">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="N42">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="O42">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="P42">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="Q42">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="R42">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="S42">
         <v>22</v>
       </c>
       <c r="T42">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="U42">
         <v>27</v>
       </c>
       <c r="V42">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="W42">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="X42">
+        <v>66</v>
       </c>
       <c r="Y42">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Z42">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="AB42">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="AC42">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="AD42">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="AE42">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="AF42">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="AG42">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="AH42">
+        <v>7</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6600102477</t>
+          <t>6600102446</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>02</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>GRUPO EMI</t>
+          <t>CAJA COLOMBIANA DE SUBSIDIO FAMILIAR COLSUBSIDIO</t>
         </is>
       </c>
       <c r="D43">
-        <v>224</v>
+        <v>30</v>
       </c>
       <c r="E43">
-        <v>353</v>
+        <v>52</v>
       </c>
       <c r="F43">
-        <v>289</v>
+        <v>58</v>
       </c>
       <c r="G43">
-        <v>243</v>
+        <v>39</v>
+      </c>
+      <c r="H43">
+        <v>29</v>
       </c>
       <c r="I43">
-        <v>151</v>
+        <v>24</v>
       </c>
       <c r="J43">
-        <v>145</v>
+        <v>27</v>
       </c>
       <c r="K43">
-        <v>228</v>
+        <v>23</v>
       </c>
       <c r="L43">
-        <v>208</v>
+        <v>26</v>
       </c>
       <c r="M43">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="N43">
-        <v>252</v>
+        <v>47</v>
       </c>
       <c r="O43">
-        <v>197</v>
+        <v>44</v>
       </c>
       <c r="P43">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="Q43">
-        <v>151</v>
+        <v>40</v>
       </c>
       <c r="R43">
-        <v>216</v>
+        <v>62</v>
       </c>
       <c r="S43">
-        <v>163</v>
+        <v>22</v>
       </c>
       <c r="T43">
-        <v>169</v>
+        <v>26</v>
       </c>
       <c r="U43">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="V43">
-        <v>192</v>
-      </c>
-      <c r="X43">
-        <v>146</v>
+        <v>25</v>
+      </c>
+      <c r="W43">
+        <v>25</v>
       </c>
       <c r="Y43">
-        <v>415</v>
+        <v>75</v>
       </c>
       <c r="Z43">
-        <v>219</v>
-      </c>
-      <c r="AA43">
-        <v>212</v>
+        <v>33</v>
       </c>
       <c r="AB43">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="AC43">
-        <v>241</v>
+        <v>27</v>
+      </c>
+      <c r="AD43">
+        <v>21</v>
       </c>
       <c r="AE43">
-        <v>201</v>
+        <v>26</v>
       </c>
       <c r="AF43">
-        <v>190</v>
+        <v>26</v>
       </c>
       <c r="AG43">
-        <v>196</v>
+        <v>29</v>
+      </c>
+      <c r="AH43">
+        <v>29</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6600102601</t>
+          <t>6600102477</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -4005,98 +4028,89 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>VIRREY SOLIS SA PINARES</t>
+          <t>GRUPO EMI</t>
         </is>
       </c>
       <c r="D44">
-        <v>33</v>
+        <v>224</v>
       </c>
       <c r="E44">
-        <v>88</v>
+        <v>353</v>
       </c>
       <c r="F44">
-        <v>120</v>
+        <v>289</v>
       </c>
       <c r="G44">
+        <v>243</v>
+      </c>
+      <c r="I44">
+        <v>151</v>
+      </c>
+      <c r="J44">
+        <v>145</v>
+      </c>
+      <c r="K44">
+        <v>228</v>
+      </c>
+      <c r="L44">
+        <v>208</v>
+      </c>
+      <c r="M44">
+        <v>227</v>
+      </c>
+      <c r="N44">
+        <v>252</v>
+      </c>
+      <c r="O44">
+        <v>197</v>
+      </c>
+      <c r="P44">
         <v>113</v>
       </c>
-      <c r="H44">
-        <v>80</v>
-      </c>
-      <c r="I44">
-        <v>89</v>
-      </c>
-      <c r="J44">
-        <v>60</v>
-      </c>
-      <c r="K44">
-        <v>117</v>
-      </c>
-      <c r="L44">
-        <v>92</v>
-      </c>
-      <c r="M44">
-        <v>89</v>
-      </c>
-      <c r="N44">
-        <v>110</v>
-      </c>
-      <c r="O44">
-        <v>74</v>
-      </c>
-      <c r="P44">
-        <v>56</v>
-      </c>
       <c r="Q44">
-        <v>107</v>
+        <v>151</v>
       </c>
       <c r="R44">
-        <v>109</v>
+        <v>216</v>
       </c>
       <c r="S44">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="T44">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="U44">
-        <v>57</v>
+        <v>153</v>
       </c>
       <c r="V44">
-        <v>91</v>
-      </c>
-      <c r="W44">
-        <v>87</v>
+        <v>192</v>
       </c>
       <c r="X44">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="Y44">
-        <v>73</v>
+        <v>415</v>
       </c>
       <c r="Z44">
-        <v>70</v>
+        <v>219</v>
       </c>
       <c r="AA44">
-        <v>95</v>
+        <v>212</v>
       </c>
       <c r="AB44">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="AC44">
-        <v>56</v>
-      </c>
-      <c r="AD44">
-        <v>58</v>
+        <v>241</v>
       </c>
       <c r="AE44">
-        <v>85</v>
+        <v>201</v>
       </c>
       <c r="AF44">
-        <v>89</v>
+        <v>190</v>
       </c>
       <c r="AG44">
-        <v>100</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45">
@@ -4107,103 +4121,106 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>VIRREY SOLIS IPS LAGO</t>
+          <t>VIRREY SOLIS SA PINARES</t>
         </is>
       </c>
       <c r="D45">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="E45">
-        <v>255</v>
+        <v>88</v>
       </c>
       <c r="F45">
-        <v>235</v>
+        <v>120</v>
       </c>
       <c r="G45">
-        <v>211</v>
+        <v>113</v>
       </c>
       <c r="H45">
-        <v>186</v>
+        <v>80</v>
       </c>
       <c r="I45">
-        <v>162</v>
+        <v>89</v>
       </c>
       <c r="J45">
-        <v>139</v>
+        <v>60</v>
       </c>
       <c r="K45">
-        <v>165</v>
+        <v>117</v>
       </c>
       <c r="L45">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="M45">
-        <v>168</v>
+        <v>89</v>
       </c>
       <c r="N45">
-        <v>186</v>
+        <v>110</v>
       </c>
       <c r="O45">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="P45">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="Q45">
-        <v>191</v>
+        <v>107</v>
       </c>
       <c r="R45">
-        <v>209</v>
+        <v>109</v>
       </c>
       <c r="S45">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="T45">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="U45">
-        <v>302</v>
+        <v>57</v>
       </c>
       <c r="V45">
-        <v>153</v>
+        <v>91</v>
       </c>
       <c r="W45">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="X45">
-        <v>326</v>
+        <v>94</v>
       </c>
       <c r="Y45">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="Z45">
-        <v>146</v>
+        <v>70</v>
       </c>
       <c r="AA45">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="AB45">
-        <v>169</v>
+        <v>110</v>
       </c>
       <c r="AC45">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="AD45">
-        <v>115</v>
+        <v>58</v>
       </c>
       <c r="AE45">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="AF45">
-        <v>156</v>
+        <v>89</v>
       </c>
       <c r="AG45">
-        <v>172</v>
+        <v>100</v>
+      </c>
+      <c r="AH45">
+        <v>73</v>
       </c>
     </row>
     <row r="46">
@@ -4214,103 +4231,106 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>03</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>VIRREY SOLIS IPS SA ALPES</t>
+          <t>VIRREY SOLIS IPS LAGO</t>
         </is>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="E46">
-        <v>6</v>
+        <v>255</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>235</v>
       </c>
       <c r="G46">
-        <v>9</v>
+        <v>211</v>
       </c>
       <c r="H46">
-        <v>5</v>
+        <v>186</v>
       </c>
       <c r="I46">
-        <v>6</v>
+        <v>162</v>
       </c>
       <c r="J46">
-        <v>2</v>
+        <v>139</v>
       </c>
       <c r="K46">
-        <v>5</v>
+        <v>165</v>
       </c>
       <c r="L46">
-        <v>2</v>
+        <v>178</v>
       </c>
       <c r="M46">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="N46">
-        <v>6</v>
+        <v>186</v>
       </c>
       <c r="O46">
-        <v>7</v>
+        <v>159</v>
       </c>
       <c r="P46">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="Q46">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="R46">
-        <v>2</v>
+        <v>209</v>
       </c>
       <c r="S46">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="T46">
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="U46">
-        <v>5</v>
+        <v>302</v>
       </c>
       <c r="V46">
-        <v>5</v>
+        <v>153</v>
       </c>
       <c r="W46">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="X46">
-        <v>5</v>
+        <v>326</v>
       </c>
       <c r="Y46">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="Z46">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="AA46">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="AB46">
-        <v>2</v>
+        <v>169</v>
       </c>
       <c r="AC46">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="AD46">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="AE46">
-        <v>3</v>
+        <v>156</v>
       </c>
       <c r="AF46">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="AG46">
-        <v>6</v>
+        <v>172</v>
+      </c>
+      <c r="AH46">
+        <v>167</v>
       </c>
     </row>
     <row r="47">
@@ -4321,216 +4341,222 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>06</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>VIRREY SOLIS IPS SA LA REBECA</t>
+          <t>VIRREY SOLIS IPS SA ALPES</t>
         </is>
       </c>
       <c r="D47">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>141</v>
+        <v>6</v>
       </c>
       <c r="F47">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="G47">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="H47">
-        <v>104</v>
+        <v>5</v>
       </c>
       <c r="I47">
-        <v>106</v>
+        <v>6</v>
       </c>
       <c r="J47">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="K47">
-        <v>102</v>
+        <v>5</v>
       </c>
       <c r="L47">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="M47">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="N47">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="O47">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="P47">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="Q47">
-        <v>159</v>
+        <v>6</v>
       </c>
       <c r="R47">
-        <v>121</v>
+        <v>2</v>
       </c>
       <c r="S47">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="T47">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="U47">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="V47">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="W47">
-        <v>137</v>
+        <v>6</v>
       </c>
       <c r="X47">
-        <v>144</v>
+        <v>5</v>
       </c>
       <c r="Y47">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="Z47">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="AA47">
-        <v>118</v>
+        <v>1</v>
       </c>
       <c r="AB47">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="AC47">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="AD47">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="AE47">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="AF47">
-        <v>121</v>
+        <v>12</v>
       </c>
       <c r="AG47">
-        <v>104</v>
+        <v>6</v>
+      </c>
+      <c r="AH47">
+        <v>7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6600102793</t>
+          <t>6600102601</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>07</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>CENTRO MEDICO PEREIRA COLSANITAS</t>
+          <t>VIRREY SOLIS IPS SA LA REBECA</t>
         </is>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="F48">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="G48">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="J48">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="K48">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="L48">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="M48">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="N48">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="O48">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="P48">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="Q48">
-        <v>5</v>
+        <v>159</v>
       </c>
       <c r="R48">
-        <v>3</v>
+        <v>121</v>
       </c>
       <c r="S48">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="T48">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="U48">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="V48">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="W48">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="X48">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="Y48">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="Z48">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="AA48">
-        <v>2</v>
+        <v>118</v>
       </c>
       <c r="AB48">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="AC48">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="AD48">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="AE48">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="AF48">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="AG48">
-        <v>2</v>
+        <v>104</v>
+      </c>
+      <c r="AH48">
+        <v>167</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6600102893</t>
+          <t>6600102793</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4540,104 +4566,107 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>NEUROMEDICA SAS</t>
+          <t>CENTRO MEDICO PEREIRA COLSANITAS</t>
         </is>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M49">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q49">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z49">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB49">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AC49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AE49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AF49">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AG49">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="AH49">
+        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6600103012</t>
+          <t>6600102893</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4647,95 +4676,107 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>SPORT MEDICAL IPS GUSTAVO PORTELA SAS</t>
+          <t>NEUROMEDICA SAS</t>
         </is>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J50">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K50">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L50">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="M50">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N50">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="O50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P50">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q50">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
       </c>
       <c r="S50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U50">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="V50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X50">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y50">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="Z50">
+        <v>0</v>
       </c>
       <c r="AA50">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AB50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AC50">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AD50">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AE50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF50">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AG50">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="AH50">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6600103078</t>
+          <t>6600103012</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4745,71 +4786,98 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>COOMEVA EMERGENCIA MEDICA SERVICIO DE AMBULANCIA P</t>
-        </is>
-      </c>
-      <c r="F51">
+          <t>SPORT MEDICAL IPS GUSTAVO PORTELA SAS</t>
+        </is>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>8</v>
+      </c>
+      <c r="G51">
+        <v>6</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+      <c r="J51">
         <v>7</v>
       </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-      <c r="H51">
-        <v>1</v>
-      </c>
-      <c r="J51">
-        <v>2</v>
-      </c>
       <c r="K51">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="L51">
+        <v>11</v>
       </c>
       <c r="M51">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="N51">
+        <v>18</v>
+      </c>
+      <c r="O51">
         <v>1</v>
       </c>
       <c r="P51">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q51">
         <v>8</v>
       </c>
-      <c r="R51">
-        <v>3</v>
+      <c r="S51">
+        <v>2</v>
       </c>
       <c r="T51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U51">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="V51">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X51">
+        <v>8</v>
+      </c>
+      <c r="Y51">
+        <v>14</v>
+      </c>
+      <c r="AA51">
+        <v>12</v>
+      </c>
+      <c r="AB51">
         <v>5</v>
       </c>
-      <c r="Y51">
-        <v>4</v>
-      </c>
-      <c r="Z51">
-        <v>1</v>
-      </c>
-      <c r="AB51">
-        <v>7</v>
+      <c r="AC51">
+        <v>8</v>
       </c>
       <c r="AD51">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="AE51">
+        <v>3</v>
+      </c>
+      <c r="AF51">
+        <v>11</v>
+      </c>
+      <c r="AG51">
+        <v>2</v>
+      </c>
+      <c r="AH51">
+        <v>11</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6600103144</t>
+          <t>6600103078</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4819,104 +4887,71 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CLINICA LOS NEVADOS SAS</t>
-        </is>
-      </c>
-      <c r="D52">
-        <v>3</v>
-      </c>
-      <c r="E52">
-        <v>29</v>
+          <t>COOMEVA EMERGENCIA MEDICA SERVICIO DE AMBULANCIA P</t>
+        </is>
       </c>
       <c r="F52">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="G52">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="H52">
-        <v>36</v>
-      </c>
-      <c r="I52">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="J52">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="K52">
-        <v>70</v>
-      </c>
-      <c r="L52">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="M52">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="N52">
-        <v>71</v>
-      </c>
-      <c r="O52">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="P52">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="Q52">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="R52">
-        <v>46</v>
-      </c>
-      <c r="S52">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="T52">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="U52">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="V52">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="W52">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="X52">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="Y52">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="Z52">
-        <v>52</v>
-      </c>
-      <c r="AA52">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="AB52">
-        <v>48</v>
-      </c>
-      <c r="AC52">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="AD52">
-        <v>50</v>
-      </c>
-      <c r="AE52">
-        <v>53</v>
-      </c>
-      <c r="AF52">
-        <v>46</v>
-      </c>
-      <c r="AG52">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6600103334</t>
+          <t>6600103144</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4926,86 +4961,107 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CLINICA CENTRAL DEL EJE SAS</t>
-        </is>
+          <t>CLINICA LOS NEVADOS SAS</t>
+        </is>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>29</v>
+      </c>
+      <c r="F53">
+        <v>60</v>
+      </c>
+      <c r="G53">
+        <v>51</v>
+      </c>
+      <c r="H53">
+        <v>36</v>
+      </c>
+      <c r="I53">
+        <v>39</v>
       </c>
       <c r="J53">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="K53">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="L53">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M53">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N53">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="O53">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="P53">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="Q53">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="R53">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="S53">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="T53">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="U53">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="V53">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="W53">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="X53">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="Y53">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="Z53">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="AA53">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AB53">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="AC53">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AD53">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="AE53">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="AF53">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="AG53">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="AH53">
+        <v>76</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6600103414</t>
+          <t>6600103334</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -5015,8 +5071,41 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CLINICA MEDICA TURIN SAS</t>
-        </is>
+          <t>CLINICA CENTRAL DEL EJE SAS</t>
+        </is>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>0</v>
       </c>
       <c r="U54">
         <v>0</v>
@@ -5025,10 +5114,10 @@
         <v>0</v>
       </c>
       <c r="W54">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y54">
         <v>0</v>
@@ -5040,13 +5129,13 @@
         <v>0</v>
       </c>
       <c r="AB54">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AC54">
         <v>0</v>
       </c>
       <c r="AD54">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE54">
         <v>0</v>
@@ -5056,315 +5145,386 @@
       </c>
       <c r="AG54">
         <v>0</v>
+      </c>
+      <c r="AH54">
+        <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6600161600</t>
+          <t>6600103414</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>01</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>EPMSC PEREIRA</t>
-        </is>
-      </c>
-      <c r="D55">
-        <v>4</v>
-      </c>
-      <c r="E55">
-        <v>4</v>
-      </c>
-      <c r="G55">
-        <v>4</v>
-      </c>
-      <c r="H55">
-        <v>3</v>
-      </c>
-      <c r="I55">
-        <v>3</v>
-      </c>
-      <c r="J55">
-        <v>4</v>
-      </c>
-      <c r="K55">
-        <v>5</v>
-      </c>
-      <c r="L55">
-        <v>8</v>
-      </c>
-      <c r="M55">
-        <v>3</v>
-      </c>
-      <c r="N55">
-        <v>3</v>
-      </c>
-      <c r="O55">
-        <v>6</v>
-      </c>
-      <c r="P55">
-        <v>6</v>
-      </c>
-      <c r="Q55">
-        <v>7</v>
-      </c>
-      <c r="R55">
-        <v>12</v>
-      </c>
-      <c r="S55">
-        <v>9</v>
-      </c>
-      <c r="T55">
-        <v>6</v>
+          <t>CLINICA MEDICA TURIN SAS</t>
+        </is>
       </c>
       <c r="U55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V55">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z55">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA55">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AB55">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC55">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AD55">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE55">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AF55">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AG55">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="AH55">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6600171151</t>
+          <t>6600161600</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>99</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SANIDAD POLICIA NACIONAL RISARALDA</t>
+          <t>EPMSC PEREIRA</t>
         </is>
       </c>
       <c r="D56">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E56">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="G56">
-        <v>93</v>
+        <v>4</v>
       </c>
       <c r="H56">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="I56">
+        <v>3</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+      <c r="K56">
+        <v>5</v>
+      </c>
+      <c r="L56">
+        <v>8</v>
+      </c>
+      <c r="M56">
+        <v>3</v>
+      </c>
+      <c r="N56">
+        <v>3</v>
+      </c>
+      <c r="O56">
+        <v>6</v>
+      </c>
+      <c r="P56">
+        <v>6</v>
+      </c>
+      <c r="Q56">
+        <v>7</v>
+      </c>
+      <c r="R56">
         <v>12</v>
       </c>
-      <c r="J56">
-        <v>90</v>
-      </c>
-      <c r="K56">
-        <v>4</v>
-      </c>
-      <c r="M56">
-        <v>271</v>
-      </c>
-      <c r="N56">
-        <v>29</v>
-      </c>
-      <c r="O56">
-        <v>35</v>
-      </c>
-      <c r="P56">
-        <v>30</v>
-      </c>
-      <c r="Q56">
-        <v>43</v>
-      </c>
       <c r="S56">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="T56">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="U56">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="V56">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="W56">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="X56">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="Y56">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="Z56">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AA56">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AB56">
-        <v>218</v>
+        <v>3</v>
       </c>
       <c r="AC56">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="AD56">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="AE56">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="AF56">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="AG56">
-        <v>55</v>
+        <v>11</v>
+      </c>
+      <c r="AH56">
+        <v>4</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>6600171151</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>SANIDAD POLICIA NACIONAL RISARALDA</t>
+        </is>
+      </c>
+      <c r="D57">
+        <v>19</v>
+      </c>
+      <c r="E57">
+        <v>45</v>
+      </c>
+      <c r="G57">
+        <v>93</v>
+      </c>
+      <c r="H57">
+        <v>22</v>
+      </c>
+      <c r="I57">
+        <v>12</v>
+      </c>
+      <c r="J57">
+        <v>90</v>
+      </c>
+      <c r="K57">
+        <v>4</v>
+      </c>
+      <c r="M57">
+        <v>271</v>
+      </c>
+      <c r="N57">
+        <v>29</v>
+      </c>
+      <c r="O57">
+        <v>35</v>
+      </c>
+      <c r="P57">
+        <v>30</v>
+      </c>
+      <c r="Q57">
+        <v>43</v>
+      </c>
+      <c r="S57">
+        <v>12</v>
+      </c>
+      <c r="T57">
+        <v>22</v>
+      </c>
+      <c r="U57">
+        <v>22</v>
+      </c>
+      <c r="V57">
+        <v>14</v>
+      </c>
+      <c r="W57">
+        <v>17</v>
+      </c>
+      <c r="X57">
+        <v>35</v>
+      </c>
+      <c r="Y57">
+        <v>19</v>
+      </c>
+      <c r="Z57">
+        <v>14</v>
+      </c>
+      <c r="AA57">
+        <v>0</v>
+      </c>
+      <c r="AB57">
+        <v>218</v>
+      </c>
+      <c r="AC57">
+        <v>100</v>
+      </c>
+      <c r="AD57">
+        <v>18</v>
+      </c>
+      <c r="AE57">
+        <v>13</v>
+      </c>
+      <c r="AF57">
+        <v>74</v>
+      </c>
+      <c r="AG57">
+        <v>55</v>
+      </c>
+      <c r="AH57">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>6600183029</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B58" t="inlineStr">
         <is>
           <t>80</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>BATALLON SAN MATEO</t>
         </is>
       </c>
-      <c r="D57">
+      <c r="D58">
         <v>10</v>
       </c>
-      <c r="E57">
+      <c r="E58">
         <v>16</v>
       </c>
-      <c r="F57">
+      <c r="F58">
         <v>61</v>
       </c>
-      <c r="G57">
+      <c r="G58">
         <v>29</v>
       </c>
-      <c r="H57">
+      <c r="H58">
         <v>15</v>
       </c>
-      <c r="I57">
+      <c r="I58">
         <v>42</v>
       </c>
-      <c r="J57">
+      <c r="J58">
         <v>42</v>
       </c>
-      <c r="K57">
+      <c r="K58">
         <v>40</v>
       </c>
-      <c r="L57">
+      <c r="L58">
         <v>45</v>
       </c>
-      <c r="M57">
+      <c r="M58">
         <v>33</v>
       </c>
-      <c r="N57">
+      <c r="N58">
         <v>25</v>
       </c>
-      <c r="O57">
+      <c r="O58">
         <v>31</v>
       </c>
-      <c r="P57">
+      <c r="P58">
         <v>37</v>
       </c>
-      <c r="Q57">
+      <c r="Q58">
         <v>39</v>
       </c>
-      <c r="R57">
+      <c r="R58">
         <v>36</v>
       </c>
-      <c r="S57">
+      <c r="S58">
         <v>43</v>
       </c>
-      <c r="T57">
+      <c r="T58">
         <v>58</v>
       </c>
-      <c r="U57">
+      <c r="U58">
         <v>33</v>
       </c>
-      <c r="V57">
+      <c r="V58">
         <v>46</v>
       </c>
-      <c r="W57">
+      <c r="W58">
         <v>23</v>
       </c>
-      <c r="X57">
+      <c r="X58">
         <v>41</v>
       </c>
-      <c r="Y57">
+      <c r="Y58">
         <v>31</v>
       </c>
-      <c r="Z57">
+      <c r="Z58">
         <v>33</v>
       </c>
-      <c r="AA57">
+      <c r="AA58">
         <v>37</v>
       </c>
-      <c r="AB57">
+      <c r="AB58">
         <v>47</v>
       </c>
-      <c r="AC57">
+      <c r="AC58">
         <v>43</v>
       </c>
-      <c r="AD57">
+      <c r="AD58">
         <v>23</v>
       </c>
-      <c r="AE57">
+      <c r="AE58">
         <v>36</v>
       </c>
-      <c r="AF57">
+      <c r="AF58">
         <v>19</v>
       </c>
-      <c r="AG57">
+      <c r="AG58">
         <v>37</v>
+      </c>
+      <c r="AH58">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
envio preliminar IRA 42 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/revision_IRAExt_semanal.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/revision_IRAExt_semanal.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR58"/>
+  <dimension ref="A1:AS58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -578,6 +578,11 @@
           <t>41</t>
         </is>
       </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -718,6 +723,9 @@
       <c r="AR2">
         <v>59</v>
       </c>
+      <c r="AS2">
+        <v>43</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -828,6 +836,9 @@
       <c r="AQ3">
         <v>68</v>
       </c>
+      <c r="AS3">
+        <v>46</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -952,7 +963,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CENTRO MEDICO Y ODONTOLOGICO DE LA CIRCUNVALAR</t>
+          <t>CAJA DE COMPENSACION FAMILIAR DE RISARALDA COMFAMI</t>
         </is>
       </c>
       <c r="D5">
@@ -1077,6 +1088,9 @@
       </c>
       <c r="AR5">
         <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -1092,7 +1106,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CLINICA COMFAMILIAR</t>
+          <t>CAJA DE COMPENSACION FAMILIAR DE RISARALDA COMFAMI</t>
         </is>
       </c>
       <c r="D6">
@@ -1355,6 +1369,9 @@
       <c r="AR7">
         <v>23</v>
       </c>
+      <c r="AS7">
+        <v>19</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1492,6 +1509,9 @@
       <c r="AR8">
         <v>18</v>
       </c>
+      <c r="AS8">
+        <v>33</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1617,6 +1637,9 @@
       <c r="AR9">
         <v>5</v>
       </c>
+      <c r="AS9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1736,6 +1759,9 @@
       <c r="AQ10">
         <v>2</v>
       </c>
+      <c r="AS10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1831,6 +1857,9 @@
       <c r="AR11">
         <v>1</v>
       </c>
+      <c r="AS11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2131,6 +2160,9 @@
       <c r="AR14">
         <v>1</v>
       </c>
+      <c r="AS14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2321,6 +2353,9 @@
       <c r="AR16">
         <v>1</v>
       </c>
+      <c r="AS16">
+        <v>3</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2437,6 +2472,9 @@
       <c r="AR17">
         <v>2</v>
       </c>
+      <c r="AS17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2571,6 +2609,9 @@
       <c r="AN21">
         <v>1</v>
       </c>
+      <c r="AS21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2672,6 +2713,9 @@
       <c r="AR22">
         <v>2</v>
       </c>
+      <c r="AS22">
+        <v>5</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2791,6 +2835,9 @@
       <c r="AR23">
         <v>7</v>
       </c>
+      <c r="AS23">
+        <v>7</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2862,6 +2909,9 @@
       <c r="AR24">
         <v>1</v>
       </c>
+      <c r="AS24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3002,6 +3052,9 @@
       <c r="AR25">
         <v>23</v>
       </c>
+      <c r="AS25">
+        <v>24</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3281,6 +3334,12 @@
       <c r="AQ28">
         <v>218</v>
       </c>
+      <c r="AR28">
+        <v>210</v>
+      </c>
+      <c r="AS28">
+        <v>163</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3418,6 +3477,9 @@
       <c r="AR29">
         <v>0</v>
       </c>
+      <c r="AS29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3555,6 +3617,9 @@
       <c r="AR30">
         <v>60</v>
       </c>
+      <c r="AS30">
+        <v>55</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3695,6 +3760,9 @@
       <c r="AR31">
         <v>3</v>
       </c>
+      <c r="AS31">
+        <v>3</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4170,6 +4238,9 @@
       <c r="AR36">
         <v>2</v>
       </c>
+      <c r="AS36">
+        <v>2</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4307,6 +4378,9 @@
       <c r="AR37">
         <v>3</v>
       </c>
+      <c r="AS37">
+        <v>12</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4447,6 +4521,9 @@
       <c r="AR38">
         <v>83</v>
       </c>
+      <c r="AS38">
+        <v>88</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4660,6 +4737,9 @@
       <c r="AR41">
         <v>5</v>
       </c>
+      <c r="AS41">
+        <v>10</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4797,6 +4877,9 @@
       <c r="AR42">
         <v>12</v>
       </c>
+      <c r="AS42">
+        <v>28</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4931,6 +5014,9 @@
       <c r="AR43">
         <v>19</v>
       </c>
+      <c r="AS43">
+        <v>24</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4945,7 +5031,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>GRUPO EMI</t>
+          <t>EMPRESA DE MEDICINA INTEGRAL EMI SA - SERVICIO DE</t>
         </is>
       </c>
       <c r="D44">
@@ -5193,6 +5279,9 @@
       <c r="AR45">
         <v>68</v>
       </c>
+      <c r="AS45">
+        <v>59</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5333,6 +5422,9 @@
       <c r="AR46">
         <v>88</v>
       </c>
+      <c r="AS46">
+        <v>75</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5473,6 +5565,9 @@
       <c r="AR47">
         <v>0</v>
       </c>
+      <c r="AS47">
+        <v>3</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5613,6 +5708,9 @@
       <c r="AR48">
         <v>104</v>
       </c>
+      <c r="AS48">
+        <v>38</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -5753,6 +5851,9 @@
       <c r="AR49">
         <v>5</v>
       </c>
+      <c r="AS49">
+        <v>3</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5893,6 +5994,9 @@
       <c r="AR50">
         <v>0</v>
       </c>
+      <c r="AS50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -6024,6 +6128,9 @@
       <c r="AR51">
         <v>11</v>
       </c>
+      <c r="AS51">
+        <v>4</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -6256,6 +6363,9 @@
       <c r="AR53">
         <v>11</v>
       </c>
+      <c r="AS53">
+        <v>9</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -6378,6 +6488,9 @@
       <c r="AR54">
         <v>0</v>
       </c>
+      <c r="AS54">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -6467,6 +6580,9 @@
       <c r="AR55">
         <v>0</v>
       </c>
+      <c r="AS55">
+        <v>2</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -6604,6 +6720,9 @@
       <c r="AR56">
         <v>10</v>
       </c>
+      <c r="AS56">
+        <v>3</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -6732,6 +6851,9 @@
       <c r="AR57">
         <v>39</v>
       </c>
+      <c r="AS57">
+        <v>16</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -6871,6 +6993,9 @@
       </c>
       <c r="AR58">
         <v>16</v>
+      </c>
+      <c r="AS58">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>